<commit_message>
Deploying to gh-pages from @ wanghuaijin/wanghuaijin.github.io@8979d20d1aefff6a027fbc8d3c64ed89fd21f275 🚀
</commit_message>
<xml_diff>
--- a/assets/numDEs/status/homework.xlsx
+++ b/assets/numDEs/status/homework.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="524">
   <si>
     <t>序号</t>
   </si>
@@ -1314,12 +1314,6 @@
     <t>√</t>
   </si>
   <si>
-    <t>Ｏ</t>
-  </si>
-  <si>
-    <t>√</t>
-  </si>
-  <si>
     <t>第15周</t>
   </si>
   <si>
@@ -1480,9 +1474,6 @@
   </si>
   <si>
     <t>93%</t>
-  </si>
-  <si>
-    <t>82%</t>
   </si>
   <si>
     <t>87%</t>
@@ -1727,19 +1718,19 @@
         <v>412</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="U1" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="W1" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="X1" s="0" t="s">
         <v>455</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>456</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="2">
@@ -1801,13 +1792,13 @@
         <v>413</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U2" s="0"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3">
@@ -1869,13 +1860,13 @@
         <v>413</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U3" s="0"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4">
@@ -1937,13 +1928,13 @@
         <v>413</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U4" s="0"/>
       <c r="V4" s="0"/>
       <c r="W4" s="0"/>
       <c r="X4" s="0" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5">
@@ -2005,13 +1996,13 @@
         <v>413</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U5" s="0"/>
       <c r="V5" s="0"/>
       <c r="W5" s="0"/>
       <c r="X5" s="0" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6">
@@ -2073,13 +2064,13 @@
         <v>413</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U6" s="0"/>
       <c r="V6" s="0"/>
       <c r="W6" s="0"/>
       <c r="X6" s="0" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7">
@@ -2141,13 +2132,13 @@
         <v>413</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U7" s="0"/>
       <c r="V7" s="0"/>
       <c r="W7" s="0"/>
       <c r="X7" s="0" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8">
@@ -2209,13 +2200,13 @@
         <v>413</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U8" s="0"/>
       <c r="V8" s="0"/>
       <c r="W8" s="0"/>
       <c r="X8" s="0" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9">
@@ -2277,13 +2268,13 @@
         <v>413</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U9" s="0"/>
       <c r="V9" s="0"/>
       <c r="W9" s="0"/>
       <c r="X9" s="0" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="10">
@@ -2345,13 +2336,13 @@
         <v>413</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U10" s="0"/>
       <c r="V10" s="0"/>
       <c r="W10" s="0"/>
       <c r="X10" s="0" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11">
@@ -2413,13 +2404,13 @@
         <v>413</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U11" s="0"/>
       <c r="V11" s="0"/>
       <c r="W11" s="0"/>
       <c r="X11" s="0" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12">
@@ -2481,13 +2472,13 @@
         <v>413</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="U12" s="0"/>
       <c r="V12" s="0"/>
       <c r="W12" s="0"/>
       <c r="X12" s="0" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="13">
@@ -2549,13 +2540,13 @@
         <v>413</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="U13" s="0"/>
       <c r="V13" s="0"/>
       <c r="W13" s="0"/>
       <c r="X13" s="0" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="14">
@@ -2617,13 +2608,13 @@
         <v>413</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U14" s="0"/>
       <c r="V14" s="0"/>
       <c r="W14" s="0"/>
       <c r="X14" s="0" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="15">
@@ -2685,13 +2676,13 @@
         <v>413</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U15" s="0"/>
       <c r="V15" s="0"/>
       <c r="W15" s="0"/>
       <c r="X15" s="0" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="16">
@@ -2753,13 +2744,13 @@
         <v>413</v>
       </c>
       <c r="T16" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U16" s="0"/>
       <c r="V16" s="0"/>
       <c r="W16" s="0"/>
       <c r="X16" s="0" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="17">
@@ -2821,13 +2812,13 @@
         <v>413</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U17" s="0"/>
       <c r="V17" s="0"/>
       <c r="W17" s="0"/>
       <c r="X17" s="0" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18">
@@ -2889,13 +2880,13 @@
         <v>413</v>
       </c>
       <c r="T18" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U18" s="0"/>
       <c r="V18" s="0"/>
       <c r="W18" s="0"/>
       <c r="X18" s="0" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="19">
@@ -2957,13 +2948,13 @@
         <v>413</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U19" s="0"/>
       <c r="V19" s="0"/>
       <c r="W19" s="0"/>
       <c r="X19" s="0" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="20">
@@ -3025,13 +3016,13 @@
         <v>413</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U20" s="0"/>
       <c r="V20" s="0"/>
       <c r="W20" s="0"/>
       <c r="X20" s="0" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21">
@@ -3093,13 +3084,13 @@
         <v>414</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U21" s="0"/>
       <c r="V21" s="0"/>
       <c r="W21" s="0"/>
       <c r="X21" s="0" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22">
@@ -3161,13 +3152,13 @@
         <v>415</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="U22" s="0"/>
       <c r="V22" s="0"/>
       <c r="W22" s="0"/>
       <c r="X22" s="0" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23">
@@ -3229,13 +3220,13 @@
         <v>416</v>
       </c>
       <c r="T23" s="0" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="U23" s="0"/>
       <c r="V23" s="0"/>
       <c r="W23" s="0"/>
       <c r="X23" s="0" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24">
@@ -3297,13 +3288,13 @@
         <v>417</v>
       </c>
       <c r="T24" s="0" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="U24" s="0"/>
       <c r="V24" s="0"/>
       <c r="W24" s="0"/>
       <c r="X24" s="0" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="25">
@@ -3365,13 +3356,13 @@
         <v>417</v>
       </c>
       <c r="T25" s="0" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="U25" s="0"/>
       <c r="V25" s="0"/>
       <c r="W25" s="0"/>
       <c r="X25" s="0" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="26">
@@ -3433,13 +3424,13 @@
         <v>417</v>
       </c>
       <c r="T26" s="0" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="U26" s="0"/>
       <c r="V26" s="0"/>
       <c r="W26" s="0"/>
       <c r="X26" s="0" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="27">
@@ -3501,13 +3492,13 @@
         <v>418</v>
       </c>
       <c r="T27" s="0" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="U27" s="0"/>
       <c r="V27" s="0"/>
       <c r="W27" s="0"/>
       <c r="X27" s="0" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="28">
@@ -3569,13 +3560,13 @@
         <v>418</v>
       </c>
       <c r="T28" s="0" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="U28" s="0"/>
       <c r="V28" s="0"/>
       <c r="W28" s="0"/>
       <c r="X28" s="0" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29">
@@ -3637,13 +3628,13 @@
         <v>419</v>
       </c>
       <c r="T29" s="0" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="U29" s="0"/>
       <c r="V29" s="0"/>
       <c r="W29" s="0"/>
       <c r="X29" s="0" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30">
@@ -3705,13 +3696,13 @@
         <v>420</v>
       </c>
       <c r="T30" s="0" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="U30" s="0"/>
       <c r="V30" s="0"/>
       <c r="W30" s="0"/>
       <c r="X30" s="0" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31">
@@ -3773,13 +3764,13 @@
         <v>421</v>
       </c>
       <c r="T31" s="0" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="U31" s="0"/>
       <c r="V31" s="0"/>
       <c r="W31" s="0"/>
       <c r="X31" s="0" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="32">
@@ -3841,13 +3832,13 @@
         <v>422</v>
       </c>
       <c r="T32" s="0" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="U32" s="0"/>
       <c r="V32" s="0"/>
       <c r="W32" s="0"/>
       <c r="X32" s="0" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="33">
@@ -3906,16 +3897,16 @@
         <v>403</v>
       </c>
       <c r="S33" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T33" s="0" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="U33" s="0"/>
       <c r="V33" s="0"/>
       <c r="W33" s="0"/>
       <c r="X33" s="0" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="34">
@@ -3974,16 +3965,16 @@
         <v>403</v>
       </c>
       <c r="S34" s="0" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="T34" s="0" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="U34" s="0"/>
       <c r="V34" s="0"/>
       <c r="W34" s="0"/>
       <c r="X34" s="0" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="35">
@@ -4042,16 +4033,16 @@
         <v>403</v>
       </c>
       <c r="S35" s="0" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="T35" s="0" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="U35" s="0"/>
       <c r="V35" s="0"/>
       <c r="W35" s="0"/>
       <c r="X35" s="0" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="36">
@@ -4110,16 +4101,16 @@
         <v>403</v>
       </c>
       <c r="S36" s="0" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="T36" s="0" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="U36" s="0"/>
       <c r="V36" s="0"/>
       <c r="W36" s="0"/>
       <c r="X36" s="0" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="37">
@@ -4178,16 +4169,16 @@
         <v>403</v>
       </c>
       <c r="S37" s="0" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="T37" s="0" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="U37" s="0"/>
       <c r="V37" s="0"/>
       <c r="W37" s="0"/>
       <c r="X37" s="0" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="38">
@@ -4246,16 +4237,16 @@
         <v>403</v>
       </c>
       <c r="S38" s="0" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="T38" s="0" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="U38" s="0"/>
       <c r="V38" s="0"/>
       <c r="W38" s="0"/>
       <c r="X38" s="0" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="39">
@@ -4314,16 +4305,16 @@
         <v>403</v>
       </c>
       <c r="S39" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T39" s="0" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="U39" s="0"/>
       <c r="V39" s="0"/>
       <c r="W39" s="0"/>
       <c r="X39" s="0" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="40">
@@ -4382,16 +4373,16 @@
         <v>403</v>
       </c>
       <c r="S40" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T40" s="0" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="U40" s="0"/>
       <c r="V40" s="0"/>
       <c r="W40" s="0"/>
       <c r="X40" s="0" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="41">
@@ -4450,16 +4441,16 @@
         <v>403</v>
       </c>
       <c r="S41" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T41" s="0" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="U41" s="0"/>
       <c r="V41" s="0"/>
       <c r="W41" s="0"/>
       <c r="X41" s="0" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="42">
@@ -4518,16 +4509,16 @@
         <v>403</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T42" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U42" s="0"/>
       <c r="V42" s="0"/>
       <c r="W42" s="0"/>
       <c r="X42" s="0" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="43">
@@ -4586,16 +4577,16 @@
         <v>403</v>
       </c>
       <c r="S43" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T43" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U43" s="0"/>
       <c r="V43" s="0"/>
       <c r="W43" s="0"/>
       <c r="X43" s="0" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="44">
@@ -4654,16 +4645,16 @@
         <v>403</v>
       </c>
       <c r="S44" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T44" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U44" s="0"/>
       <c r="V44" s="0"/>
       <c r="W44" s="0"/>
       <c r="X44" s="0" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="45">
@@ -4722,16 +4713,16 @@
         <v>403</v>
       </c>
       <c r="S45" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T45" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U45" s="0"/>
       <c r="V45" s="0"/>
       <c r="W45" s="0"/>
       <c r="X45" s="0" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="46">
@@ -4790,16 +4781,16 @@
         <v>403</v>
       </c>
       <c r="S46" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T46" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U46" s="0"/>
       <c r="V46" s="0"/>
       <c r="W46" s="0"/>
       <c r="X46" s="0" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="47">
@@ -4858,16 +4849,16 @@
         <v>403</v>
       </c>
       <c r="S47" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T47" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U47" s="0"/>
       <c r="V47" s="0"/>
       <c r="W47" s="0"/>
       <c r="X47" s="0" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="48">
@@ -4926,16 +4917,16 @@
         <v>403</v>
       </c>
       <c r="S48" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T48" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U48" s="0"/>
       <c r="V48" s="0"/>
       <c r="W48" s="0"/>
       <c r="X48" s="0" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="49">
@@ -4994,16 +4985,16 @@
         <v>403</v>
       </c>
       <c r="S49" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T49" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U49" s="0"/>
       <c r="V49" s="0"/>
       <c r="W49" s="0"/>
       <c r="X49" s="0" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="50">
@@ -5062,16 +5053,16 @@
         <v>403</v>
       </c>
       <c r="S50" s="0" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="T50" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U50" s="0"/>
       <c r="V50" s="0"/>
       <c r="W50" s="0"/>
       <c r="X50" s="0" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="51">
@@ -5130,16 +5121,16 @@
         <v>403</v>
       </c>
       <c r="S51" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T51" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U51" s="0"/>
       <c r="V51" s="0"/>
       <c r="W51" s="0"/>
       <c r="X51" s="0" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="52">
@@ -5198,16 +5189,16 @@
         <v>403</v>
       </c>
       <c r="S52" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T52" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U52" s="0"/>
       <c r="V52" s="0"/>
       <c r="W52" s="0"/>
       <c r="X52" s="0" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="53">
@@ -5266,16 +5257,16 @@
         <v>403</v>
       </c>
       <c r="S53" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T53" s="0" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U53" s="0"/>
       <c r="V53" s="0"/>
       <c r="W53" s="0"/>
       <c r="X53" s="0" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="54">
@@ -5334,16 +5325,16 @@
         <v>404</v>
       </c>
       <c r="S54" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T54" s="0" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="U54" s="0"/>
       <c r="V54" s="0"/>
       <c r="W54" s="0"/>
       <c r="X54" s="0" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="55">
@@ -5402,16 +5393,16 @@
         <v>405</v>
       </c>
       <c r="S55" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T55" s="0" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="U55" s="0"/>
       <c r="V55" s="0"/>
       <c r="W55" s="0"/>
       <c r="X55" s="0" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="56">
@@ -5470,16 +5461,16 @@
         <v>406</v>
       </c>
       <c r="S56" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T56" s="0" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="U56" s="0"/>
       <c r="V56" s="0"/>
       <c r="W56" s="0"/>
       <c r="X56" s="0" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="57">
@@ -5538,16 +5529,16 @@
         <v>407</v>
       </c>
       <c r="S57" s="0" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="T57" s="0" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="U57" s="0"/>
       <c r="V57" s="0"/>
       <c r="W57" s="0"/>
       <c r="X57" s="0" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="58">
@@ -5606,16 +5597,16 @@
         <v>408</v>
       </c>
       <c r="S58" s="0" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="T58" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U58" s="0"/>
       <c r="V58" s="0"/>
       <c r="W58" s="0"/>
       <c r="X58" s="0" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="59">
@@ -5674,16 +5665,16 @@
         <v>409</v>
       </c>
       <c r="S59" s="0" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="T59" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U59" s="0"/>
       <c r="V59" s="0"/>
       <c r="W59" s="0"/>
       <c r="X59" s="0" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="60">
@@ -5742,16 +5733,16 @@
         <v>409</v>
       </c>
       <c r="S60" s="0" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="T60" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U60" s="0"/>
       <c r="V60" s="0"/>
       <c r="W60" s="0"/>
       <c r="X60" s="0" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="61">
@@ -5810,16 +5801,16 @@
         <v>409</v>
       </c>
       <c r="S61" s="0" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="T61" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U61" s="0"/>
       <c r="V61" s="0"/>
       <c r="W61" s="0"/>
       <c r="X61" s="0" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="62">
@@ -5878,16 +5869,16 @@
         <v>409</v>
       </c>
       <c r="S62" s="0" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="T62" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U62" s="0"/>
       <c r="V62" s="0"/>
       <c r="W62" s="0"/>
       <c r="X62" s="0" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="63">
@@ -5946,16 +5937,16 @@
         <v>410</v>
       </c>
       <c r="S63" s="0" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="T63" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U63" s="0"/>
       <c r="V63" s="0"/>
       <c r="W63" s="0"/>
       <c r="X63" s="0" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="64">
@@ -6014,16 +6005,16 @@
         <v>411</v>
       </c>
       <c r="S64" s="0" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="T64" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U64" s="0"/>
       <c r="V64" s="0"/>
       <c r="W64" s="0"/>
       <c r="X64" s="0" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="65">
@@ -6082,16 +6073,16 @@
         <v>411</v>
       </c>
       <c r="S65" s="0" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="T65" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U65" s="0"/>
       <c r="V65" s="0"/>
       <c r="W65" s="0"/>
       <c r="X65" s="0" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="66">
@@ -6150,16 +6141,16 @@
         <v>411</v>
       </c>
       <c r="S66" s="0" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="T66" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U66" s="0"/>
       <c r="V66" s="0"/>
       <c r="W66" s="0"/>
       <c r="X66" s="0" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="67">
@@ -6218,16 +6209,16 @@
         <v>411</v>
       </c>
       <c r="S67" s="0" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="T67" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U67" s="0"/>
       <c r="V67" s="0"/>
       <c r="W67" s="0"/>
       <c r="X67" s="0" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="68">
@@ -6286,16 +6277,16 @@
         <v>411</v>
       </c>
       <c r="S68" s="0" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="T68" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U68" s="0"/>
       <c r="V68" s="0"/>
       <c r="W68" s="0"/>
       <c r="X68" s="0" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="69">
@@ -6354,16 +6345,16 @@
         <v>411</v>
       </c>
       <c r="S69" s="0" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T69" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U69" s="0"/>
       <c r="V69" s="0"/>
       <c r="W69" s="0"/>
       <c r="X69" s="0" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="70">
@@ -6422,16 +6413,16 @@
         <v>411</v>
       </c>
       <c r="S70" s="0" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T70" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U70" s="0"/>
       <c r="V70" s="0"/>
       <c r="W70" s="0"/>
       <c r="X70" s="0" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="71">
@@ -6490,16 +6481,16 @@
         <v>411</v>
       </c>
       <c r="S71" s="0" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T71" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U71" s="0"/>
       <c r="V71" s="0"/>
       <c r="W71" s="0"/>
       <c r="X71" s="0" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>